<commit_message>
Correções para Dia 2
</commit_message>
<xml_diff>
--- a/Horarios.xlsx
+++ b/Horarios.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="22">
   <si>
     <t xml:space="preserve">Dias</t>
   </si>
@@ -210,7 +210,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,9 +276,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -290,9 +294,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -550,7 +558,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="E18 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="F4:F5 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -655,7 +663,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="E18 H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="F4:F5 H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>